<commit_message>
ITST-20744 - Enhance aspera/xlsx-reader - Account for rounding issue problems present in popular spreadsheet editors
- Add notes about floating point math gotchas to docs of configuration options for disabling formatting of returned values.
- Extend CellFormatConfigTest with a testcase which exhibits this problem.
</commit_message>
<xml_diff>
--- a/tests/input_files/cell_format_config_test.xlsx
+++ b/tests/input_files/cell_format_config_test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5F6DE9-173A-4D12-8FB0-A832DD89AD7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E37E1EA-C83F-4810-992B-8E0D5CCCD934}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="2985" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="1590" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date:</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Percent:</t>
+  </si>
+  <si>
+    <t>Rounding Error:</t>
   </si>
 </sst>
 </file>
@@ -353,15 +356,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -397,6 +400,14 @@
         <v>0.255</v>
       </c>
     </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>